<commit_message>
Update logging message in API helper and simplify pytest markers descriptions
</commit_message>
<xml_diff>
--- a/automation/data/userdata.xlsx
+++ b/automation/data/userdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -28,49 +28,94 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">suhas1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suhas15</t>
+    <t xml:space="preserve">alpha_user01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XyT7!pQ9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beta_user02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ab9#Lm42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gamma_user03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zt5@Kr81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delta_user04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pm2$Qh67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omega_user05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr8!Xn24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sigma_user06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hn9&amp;Pq31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">theta_user07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jk4#Zr58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zeta_user08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tb7!Yx92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kappa_user09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rc3$Uv76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lambda_user10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Df6^Wp19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mu_user11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vg2!Lq83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nu_user12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mn8&amp;St47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xi_user13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wq5@Jd62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pi_user14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kl1#Fv95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rho_user15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sb7^Gh28</t>
   </si>
 </sst>
 </file>
@@ -85,6 +130,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,6 +152,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,13 +197,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -179,10 +230,14 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B16"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.51"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -193,123 +248,123 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>2</v>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>3</v>
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>4</v>
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>5</v>
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>6</v>
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>7</v>
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>8</v>
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>9</v>
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>10</v>
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>11</v>
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>12</v>
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>13</v>
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>14</v>
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>15</v>
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>16</v>
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>